<commit_message>
form validation & font optimization
</commit_message>
<xml_diff>
--- a/public/example.xlsx
+++ b/public/example.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riswa\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\cekNikIndosat\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CD98E0E-7A85-4C0A-A940-A9DE883C1E23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF5D0254-3E97-4159-91EE-51639A3B9E7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{785CB447-F45F-4B52-A0F8-CF5E9939EEE2}"/>
   </bookViews>
@@ -47,12 +47,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -76,15 +84,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,28 +408,748 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFE1311D-64ED-42CC-8B78-8D3E4ECC8686}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B182"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.44140625" customWidth="1"/>
+    <col min="1" max="2" width="19" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B2" s="1"/>
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+    </row>
+    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+    </row>
+    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+    </row>
+    <row r="6" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+    </row>
+    <row r="8" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+    </row>
+    <row r="14" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+    </row>
+    <row r="20" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+    </row>
+    <row r="21" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+    </row>
+    <row r="23" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+    </row>
+    <row r="24" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+    </row>
+    <row r="25" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+    </row>
+    <row r="26" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+    </row>
+    <row r="27" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+    </row>
+    <row r="28" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+    </row>
+    <row r="29" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+    </row>
+    <row r="30" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+    </row>
+    <row r="31" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+    </row>
+    <row r="32" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+    </row>
+    <row r="33" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+    </row>
+    <row r="34" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+    </row>
+    <row r="35" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+    </row>
+    <row r="36" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+    </row>
+    <row r="37" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+    </row>
+    <row r="38" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+    </row>
+    <row r="39" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+    </row>
+    <row r="40" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+    </row>
+    <row r="41" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
+    </row>
+    <row r="42" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
+    </row>
+    <row r="43" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A43" s="3"/>
+      <c r="B43" s="3"/>
+    </row>
+    <row r="44" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
+    </row>
+    <row r="45" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A45" s="3"/>
+      <c r="B45" s="3"/>
+    </row>
+    <row r="46" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="3"/>
+      <c r="B46" s="3"/>
+    </row>
+    <row r="47" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="3"/>
+      <c r="B47" s="3"/>
+    </row>
+    <row r="48" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+    </row>
+    <row r="49" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A49" s="3"/>
+      <c r="B49" s="3"/>
+    </row>
+    <row r="50" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
+    </row>
+    <row r="51" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A51" s="3"/>
+      <c r="B51" s="3"/>
+    </row>
+    <row r="52" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A52" s="3"/>
+      <c r="B52" s="3"/>
+    </row>
+    <row r="53" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A53" s="3"/>
+      <c r="B53" s="3"/>
+    </row>
+    <row r="54" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A54" s="3"/>
+      <c r="B54" s="3"/>
+    </row>
+    <row r="55" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A55" s="3"/>
+      <c r="B55" s="3"/>
+    </row>
+    <row r="56" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A56" s="3"/>
+      <c r="B56" s="3"/>
+    </row>
+    <row r="57" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A57" s="3"/>
+      <c r="B57" s="3"/>
+    </row>
+    <row r="58" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A58" s="3"/>
+      <c r="B58" s="3"/>
+    </row>
+    <row r="59" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A59" s="3"/>
+      <c r="B59" s="3"/>
+    </row>
+    <row r="60" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A60" s="3"/>
+      <c r="B60" s="3"/>
+    </row>
+    <row r="61" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A61" s="3"/>
+      <c r="B61" s="3"/>
+    </row>
+    <row r="62" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A62" s="3"/>
+      <c r="B62" s="3"/>
+    </row>
+    <row r="63" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A63" s="3"/>
+      <c r="B63" s="3"/>
+    </row>
+    <row r="64" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A64" s="3"/>
+      <c r="B64" s="3"/>
+    </row>
+    <row r="65" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A65" s="3"/>
+      <c r="B65" s="3"/>
+    </row>
+    <row r="66" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A66" s="3"/>
+      <c r="B66" s="3"/>
+    </row>
+    <row r="67" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A67" s="3"/>
+      <c r="B67" s="3"/>
+    </row>
+    <row r="68" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A68" s="3"/>
+      <c r="B68" s="3"/>
+    </row>
+    <row r="69" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A69" s="3"/>
+      <c r="B69" s="3"/>
+    </row>
+    <row r="70" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A70" s="3"/>
+      <c r="B70" s="3"/>
+    </row>
+    <row r="71" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A71" s="3"/>
+      <c r="B71" s="3"/>
+    </row>
+    <row r="72" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A72" s="3"/>
+      <c r="B72" s="3"/>
+    </row>
+    <row r="73" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A73" s="3"/>
+      <c r="B73" s="3"/>
+    </row>
+    <row r="74" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A74" s="3"/>
+      <c r="B74" s="3"/>
+    </row>
+    <row r="75" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A75" s="3"/>
+      <c r="B75" s="3"/>
+    </row>
+    <row r="76" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A76" s="3"/>
+      <c r="B76" s="3"/>
+    </row>
+    <row r="77" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A77" s="3"/>
+      <c r="B77" s="3"/>
+    </row>
+    <row r="78" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A78" s="3"/>
+      <c r="B78" s="3"/>
+    </row>
+    <row r="79" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A79" s="3"/>
+      <c r="B79" s="3"/>
+    </row>
+    <row r="80" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A80" s="3"/>
+      <c r="B80" s="3"/>
+    </row>
+    <row r="81" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A81" s="3"/>
+      <c r="B81" s="3"/>
+    </row>
+    <row r="82" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A82" s="3"/>
+      <c r="B82" s="3"/>
+    </row>
+    <row r="83" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A83" s="3"/>
+      <c r="B83" s="3"/>
+    </row>
+    <row r="84" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A84" s="3"/>
+      <c r="B84" s="3"/>
+    </row>
+    <row r="85" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A85" s="3"/>
+      <c r="B85" s="3"/>
+    </row>
+    <row r="86" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A86" s="3"/>
+      <c r="B86" s="3"/>
+    </row>
+    <row r="87" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A87" s="3"/>
+      <c r="B87" s="3"/>
+    </row>
+    <row r="88" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A88" s="3"/>
+      <c r="B88" s="3"/>
+    </row>
+    <row r="89" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A89" s="3"/>
+      <c r="B89" s="3"/>
+    </row>
+    <row r="90" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A90" s="3"/>
+      <c r="B90" s="3"/>
+    </row>
+    <row r="91" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A91" s="3"/>
+      <c r="B91" s="3"/>
+    </row>
+    <row r="92" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A92" s="3"/>
+      <c r="B92" s="3"/>
+    </row>
+    <row r="93" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A93" s="3"/>
+      <c r="B93" s="3"/>
+    </row>
+    <row r="94" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A94" s="3"/>
+      <c r="B94" s="3"/>
+    </row>
+    <row r="95" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A95" s="3"/>
+      <c r="B95" s="3"/>
+    </row>
+    <row r="96" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A96" s="3"/>
+      <c r="B96" s="3"/>
+    </row>
+    <row r="97" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A97" s="3"/>
+      <c r="B97" s="3"/>
+    </row>
+    <row r="98" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A98" s="3"/>
+      <c r="B98" s="3"/>
+    </row>
+    <row r="99" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A99" s="3"/>
+      <c r="B99" s="3"/>
+    </row>
+    <row r="100" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A100" s="3"/>
+      <c r="B100" s="3"/>
+    </row>
+    <row r="101" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A101" s="3"/>
+      <c r="B101" s="3"/>
+    </row>
+    <row r="102" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A102" s="3"/>
+      <c r="B102" s="3"/>
+    </row>
+    <row r="103" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A103" s="3"/>
+      <c r="B103" s="3"/>
+    </row>
+    <row r="104" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A104" s="3"/>
+      <c r="B104" s="3"/>
+    </row>
+    <row r="105" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A105" s="3"/>
+      <c r="B105" s="3"/>
+    </row>
+    <row r="106" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A106" s="3"/>
+      <c r="B106" s="3"/>
+    </row>
+    <row r="107" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A107" s="3"/>
+      <c r="B107" s="3"/>
+    </row>
+    <row r="108" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A108" s="3"/>
+      <c r="B108" s="3"/>
+    </row>
+    <row r="109" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A109" s="3"/>
+      <c r="B109" s="3"/>
+    </row>
+    <row r="110" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A110" s="3"/>
+      <c r="B110" s="3"/>
+    </row>
+    <row r="111" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A111" s="3"/>
+      <c r="B111" s="3"/>
+    </row>
+    <row r="112" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A112" s="3"/>
+      <c r="B112" s="3"/>
+    </row>
+    <row r="113" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A113" s="3"/>
+      <c r="B113" s="3"/>
+    </row>
+    <row r="114" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A114" s="3"/>
+      <c r="B114" s="3"/>
+    </row>
+    <row r="115" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A115" s="3"/>
+      <c r="B115" s="3"/>
+    </row>
+    <row r="116" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A116" s="3"/>
+      <c r="B116" s="3"/>
+    </row>
+    <row r="117" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A117" s="3"/>
+      <c r="B117" s="3"/>
+    </row>
+    <row r="118" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A118" s="3"/>
+      <c r="B118" s="3"/>
+    </row>
+    <row r="119" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A119" s="3"/>
+      <c r="B119" s="3"/>
+    </row>
+    <row r="120" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A120" s="3"/>
+      <c r="B120" s="3"/>
+    </row>
+    <row r="121" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A121" s="3"/>
+      <c r="B121" s="3"/>
+    </row>
+    <row r="122" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A122" s="3"/>
+      <c r="B122" s="3"/>
+    </row>
+    <row r="123" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A123" s="3"/>
+      <c r="B123" s="3"/>
+    </row>
+    <row r="124" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A124" s="3"/>
+      <c r="B124" s="3"/>
+    </row>
+    <row r="125" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A125" s="3"/>
+      <c r="B125" s="3"/>
+    </row>
+    <row r="126" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A126" s="3"/>
+      <c r="B126" s="3"/>
+    </row>
+    <row r="127" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A127" s="3"/>
+      <c r="B127" s="3"/>
+    </row>
+    <row r="128" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A128" s="3"/>
+      <c r="B128" s="3"/>
+    </row>
+    <row r="129" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A129" s="3"/>
+      <c r="B129" s="3"/>
+    </row>
+    <row r="130" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A130" s="3"/>
+      <c r="B130" s="3"/>
+    </row>
+    <row r="131" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A131" s="3"/>
+      <c r="B131" s="3"/>
+    </row>
+    <row r="132" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A132" s="3"/>
+      <c r="B132" s="3"/>
+    </row>
+    <row r="133" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A133" s="3"/>
+      <c r="B133" s="3"/>
+    </row>
+    <row r="134" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A134" s="3"/>
+      <c r="B134" s="3"/>
+    </row>
+    <row r="135" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A135" s="3"/>
+      <c r="B135" s="3"/>
+    </row>
+    <row r="136" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A136" s="3"/>
+      <c r="B136" s="3"/>
+    </row>
+    <row r="137" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A137" s="3"/>
+      <c r="B137" s="3"/>
+    </row>
+    <row r="138" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A138" s="3"/>
+      <c r="B138" s="3"/>
+    </row>
+    <row r="139" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A139" s="3"/>
+      <c r="B139" s="3"/>
+    </row>
+    <row r="140" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A140" s="3"/>
+      <c r="B140" s="3"/>
+    </row>
+    <row r="141" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A141" s="3"/>
+      <c r="B141" s="3"/>
+    </row>
+    <row r="142" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A142" s="3"/>
+      <c r="B142" s="3"/>
+    </row>
+    <row r="143" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A143" s="3"/>
+      <c r="B143" s="3"/>
+    </row>
+    <row r="144" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A144" s="3"/>
+      <c r="B144" s="3"/>
+    </row>
+    <row r="145" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A145" s="3"/>
+      <c r="B145" s="3"/>
+    </row>
+    <row r="146" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A146" s="3"/>
+      <c r="B146" s="3"/>
+    </row>
+    <row r="147" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A147" s="3"/>
+      <c r="B147" s="3"/>
+    </row>
+    <row r="148" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A148" s="3"/>
+      <c r="B148" s="3"/>
+    </row>
+    <row r="149" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A149" s="3"/>
+      <c r="B149" s="3"/>
+    </row>
+    <row r="150" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A150" s="3"/>
+      <c r="B150" s="3"/>
+    </row>
+    <row r="151" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A151" s="3"/>
+      <c r="B151" s="3"/>
+    </row>
+    <row r="152" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A152" s="3"/>
+      <c r="B152" s="3"/>
+    </row>
+    <row r="153" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A153" s="3"/>
+      <c r="B153" s="3"/>
+    </row>
+    <row r="154" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A154" s="3"/>
+      <c r="B154" s="3"/>
+    </row>
+    <row r="155" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A155" s="3"/>
+      <c r="B155" s="3"/>
+    </row>
+    <row r="156" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A156" s="3"/>
+      <c r="B156" s="3"/>
+    </row>
+    <row r="157" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A157" s="3"/>
+      <c r="B157" s="3"/>
+    </row>
+    <row r="158" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A158" s="3"/>
+      <c r="B158" s="3"/>
+    </row>
+    <row r="159" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A159" s="3"/>
+      <c r="B159" s="3"/>
+    </row>
+    <row r="160" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A160" s="3"/>
+      <c r="B160" s="3"/>
+    </row>
+    <row r="161" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A161" s="3"/>
+      <c r="B161" s="3"/>
+    </row>
+    <row r="162" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A162" s="3"/>
+      <c r="B162" s="3"/>
+    </row>
+    <row r="163" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A163" s="3"/>
+      <c r="B163" s="3"/>
+    </row>
+    <row r="164" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A164" s="3"/>
+      <c r="B164" s="3"/>
+    </row>
+    <row r="165" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A165" s="3"/>
+      <c r="B165" s="3"/>
+    </row>
+    <row r="166" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A166" s="3"/>
+      <c r="B166" s="3"/>
+    </row>
+    <row r="167" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A167" s="3"/>
+      <c r="B167" s="3"/>
+    </row>
+    <row r="168" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A168" s="3"/>
+      <c r="B168" s="3"/>
+    </row>
+    <row r="169" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A169" s="3"/>
+      <c r="B169" s="3"/>
+    </row>
+    <row r="170" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A170" s="3"/>
+      <c r="B170" s="3"/>
+    </row>
+    <row r="171" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A171" s="3"/>
+      <c r="B171" s="3"/>
+    </row>
+    <row r="172" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A172" s="3"/>
+      <c r="B172" s="3"/>
+    </row>
+    <row r="173" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A173" s="3"/>
+      <c r="B173" s="3"/>
+    </row>
+    <row r="174" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A174" s="4"/>
+      <c r="B174" s="4"/>
+    </row>
+    <row r="175" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A175" s="4"/>
+      <c r="B175" s="4"/>
+    </row>
+    <row r="176" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A176" s="4"/>
+      <c r="B176" s="4"/>
+    </row>
+    <row r="177" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A177" s="4"/>
+      <c r="B177" s="4"/>
+    </row>
+    <row r="178" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A178" s="4"/>
+      <c r="B178" s="4"/>
+    </row>
+    <row r="179" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A179" s="4"/>
+      <c r="B179" s="4"/>
+    </row>
+    <row r="180" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A180" s="4"/>
+      <c r="B180" s="4"/>
+    </row>
+    <row r="181" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A181" s="4"/>
+      <c r="B181" s="4"/>
+    </row>
+    <row r="182" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A182" s="4"/>
+      <c r="B182" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>